<commit_message>
added info on ID elements
</commit_message>
<xml_diff>
--- a/identity_elements.xlsx
+++ b/identity_elements.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguppy/PycharmProjects/orthoT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amirg\Chi-T\Chi-T\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B657B9-A27D-E645-A9CF-77D943F8CC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF86108-7BF4-4099-B417-357041462DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19760" xr2:uid="{E3EA50A5-9C76-0045-B183-D4403DF8C647}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3EA50A5-9C76-0045-B183-D4403DF8C647}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <r>
       <t xml:space="preserve">Identity elements for </t>
@@ -104,9 +107,6 @@
     <t>GlyRS</t>
   </si>
   <si>
-    <t>1, 2, 3, 35, 36, 70, 71, 72, 73</t>
-  </si>
-  <si>
     <t>HisRS</t>
   </si>
   <si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t xml:space="preserve">15, 35, 36, 48, 72, 73 </t>
+  </si>
+  <si>
+    <t>19, 56, 17</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 35, 36, 37, 70, 71, 72, 73</t>
   </si>
 </sst>
 </file>
@@ -552,24 +558,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A13B15-E43C-4F4A-8A77-8283A6DAFAE0}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -577,15 +583,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -593,7 +602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -601,7 +610,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -609,7 +618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -617,7 +626,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -625,108 +634,111 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="1" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>